<commit_message>
Ajuste Formato Recolección Información
</commit_message>
<xml_diff>
--- a/app/1_app_documentacion/1er_Trim/1_3_recoleccion/1_3_1_recoleccion_informacion.xlsx
+++ b/app/1_app_documentacion/1er_Trim/1_3_recoleccion/1_3_1_recoleccion_informacion.xlsx
@@ -9,25 +9,27 @@
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
     <sheet name="Planeación" sheetId="6" r:id="rId2"/>
-    <sheet name="Instrumentos" sheetId="7" r:id="rId3"/>
-    <sheet name="Tabulación" sheetId="8" r:id="rId4"/>
-    <sheet name="Reportes Gráficos" sheetId="9" r:id="rId5"/>
-    <sheet name="Análisis" sheetId="10" r:id="rId6"/>
+    <sheet name="Técnicas" sheetId="11" r:id="rId3"/>
+    <sheet name="Instrumentos" sheetId="7" r:id="rId4"/>
+    <sheet name="Tabulación" sheetId="8" r:id="rId5"/>
+    <sheet name="Reportes Gráficos" sheetId="9" r:id="rId6"/>
+    <sheet name="Análisis" sheetId="10" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Análisis!$B$2:$F$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Análisis!$B$2:$F$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Hoja de Control'!$B$2:$F$46</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Instrumentos!$B$2:$F$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Instrumentos!$B$2:$F$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Planeación!$B$2:$F$14</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Reportes Gráficos'!$B$2:$F$14</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">Tabulación!$B$2:$F$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Reportes Gráficos'!$B$2:$F$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Tabulación!$B$2:$F$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Técnicas!$B$2:$F$14</definedName>
   </definedNames>
   <calcPr calcId="122211" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>&lt;Nombre Proyecto&gt;</t>
   </si>
@@ -129,6 +131,9 @@
   </si>
   <si>
     <t>Análisis de la Información</t>
+  </si>
+  <si>
+    <t>Técnicas de Recolección</t>
   </si>
 </sst>
 </file>
@@ -652,7 +657,20 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -678,19 +696,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_BuiltIn_Hyperlink" xfId="2"/>
@@ -814,7 +819,7 @@
     <xdr:ext cx="1458001" cy="1010155"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -906,6 +911,52 @@
     <xdr:ext cx="1458001" cy="1010155"/>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:lum bright="-50000"/>
+          <a:alphaModFix/>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1089257" y="929673"/>
+          <a:ext cx="1458001" cy="1010155"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln cap="flat">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>289157</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>24798</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1458001" cy="1010155"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Imagen 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -940,7 +991,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1301,44 +1352,44 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="2:8" ht="30">
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="2:8" ht="30">
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
     </row>
     <row r="12" spans="2:8">
       <c r="F12" s="4"/>
     </row>
     <row r="15" spans="2:8" ht="30">
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickBot="1">
       <c r="B17" s="2"/>
@@ -1349,54 +1400,54 @@
       <c r="B18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
     </row>
     <row r="19" spans="2:16" ht="18">
       <c r="B19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
     </row>
     <row r="20" spans="2:16" ht="18">
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
     </row>
     <row r="21" spans="2:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="B21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
     </row>
     <row r="22" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="46"/>
+      <c r="D22" s="53"/>
       <c r="E22" s="8" t="s">
         <v>10</v>
       </c>
@@ -1408,8 +1459,8 @@
       <c r="B23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="10" t="s">
         <v>13</v>
       </c>
@@ -1419,8 +1470,8 @@
     </row>
     <row r="24" spans="2:16" ht="36.75" thickBot="1">
       <c r="B24" s="11"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
       <c r="E24" s="12" t="s">
         <v>14</v>
       </c>
@@ -1450,10 +1501,10 @@
       <c r="C28" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="49"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="18" t="s">
         <v>20</v>
       </c>
@@ -1465,10 +1516,10 @@
       <c r="C29" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="50" t="s">
+      <c r="D29" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="50"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="21" t="s">
         <v>11</v>
       </c>
@@ -1476,57 +1527,57 @@
     <row r="30" spans="2:16" ht="25.5" customHeight="1">
       <c r="B30" s="22"/>
       <c r="C30" s="23"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="9"/>
     </row>
     <row r="31" spans="2:16" ht="25.5" customHeight="1">
       <c r="B31" s="22"/>
       <c r="C31" s="23"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
       <c r="F31" s="9"/>
     </row>
     <row r="32" spans="2:16" ht="25.5" customHeight="1">
       <c r="B32" s="22"/>
       <c r="C32" s="23"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
       <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:10" ht="25.5" customHeight="1">
       <c r="B33" s="22"/>
       <c r="C33" s="23"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
       <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:10" ht="25.5" customHeight="1">
       <c r="B34" s="22"/>
       <c r="C34" s="23"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
       <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:10" ht="25.5" customHeight="1">
       <c r="B35" s="22"/>
       <c r="C35" s="23"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:10" ht="25.5" customHeight="1">
       <c r="B36" s="22"/>
       <c r="C36" s="23"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
       <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:10" ht="25.5" customHeight="1" thickBot="1">
       <c r="B37" s="24"/>
       <c r="C37" s="25"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
       <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:10" ht="19.899999999999999" customHeight="1" thickTop="1">
@@ -1540,52 +1591,52 @@
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" thickBot="1"/>
     <row r="41" spans="1:10" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
     </row>
     <row r="42" spans="1:10" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
     </row>
     <row r="43" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
       <c r="J43" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
     </row>
     <row r="45" spans="1:10" ht="25.5" customHeight="1">
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
       <c r="G45" s="26"/>
     </row>
     <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
     </row>
     <row r="47" spans="1:10" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A47" s="27"/>
@@ -1901,11 +1952,18 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="D28:E28"/>
@@ -1918,18 +1976,11 @@
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D37:E37"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.9763779527559107E-2" bottom="3.9763779527559107E-2" header="0" footer="0"/>
@@ -1942,7 +1993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IW41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1968,32 +2019,32 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
     </row>
     <row r="12" spans="1:257">
       <c r="F12" s="4"/>
@@ -2208,7 +2259,273 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IW41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="12" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="12" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="1" customWidth="1"/>
+    <col min="13" max="256" width="12" style="1" customWidth="1"/>
+    <col min="257" max="257" width="12.5703125" style="2" customWidth="1"/>
+    <col min="258" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:257">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="5" spans="1:257">
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+    </row>
+    <row r="6" spans="1:257">
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+    </row>
+    <row r="7" spans="1:257" ht="30">
+      <c r="C7" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:257" ht="30">
+      <c r="C8" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+    </row>
+    <row r="12" spans="1:257">
+      <c r="F12" s="4"/>
+    </row>
+    <row r="15" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A15" s="31"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="26"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="IW15" s="2"/>
+    </row>
+    <row r="16" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A16" s="31"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="26"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="IW16" s="2"/>
+    </row>
+    <row r="17" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A17" s="31"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="IW17" s="2"/>
+    </row>
+    <row r="18" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A18" s="31"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="IW18" s="2"/>
+    </row>
+    <row r="19" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A19" s="31"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="IW19" s="2"/>
+    </row>
+    <row r="20" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A20" s="31"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="IW20" s="2"/>
+    </row>
+    <row r="21" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A21" s="31"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="IW21" s="2"/>
+    </row>
+    <row r="22" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A22" s="31"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="IW22" s="2"/>
+    </row>
+    <row r="23" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A23" s="31"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="IW23" s="2"/>
+    </row>
+    <row r="24" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A24" s="31"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="IW24" s="2"/>
+    </row>
+    <row r="25" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A25" s="31"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="IW25" s="2"/>
+    </row>
+    <row r="26" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A26" s="31"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="IW26" s="2"/>
+    </row>
+    <row r="27" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A27" s="31"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="IW27" s="2"/>
+    </row>
+    <row r="28" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="IW28" s="2"/>
+    </row>
+    <row r="29" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="B29" s="35"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="IW29" s="2"/>
+    </row>
+    <row r="30" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="IW30" s="2"/>
+    </row>
+    <row r="31" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="B31" s="35"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="IW31" s="2"/>
+    </row>
+    <row r="32" spans="1:257" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="J32" s="36"/>
+      <c r="IW32" s="2"/>
+    </row>
+    <row r="33" spans="2:257" s="1" customFormat="1">
+      <c r="B33" s="35"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="J33" s="36"/>
+      <c r="IW33" s="2"/>
+    </row>
+    <row r="34" spans="2:257" s="1" customFormat="1">
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="IW34" s="2"/>
+    </row>
+    <row r="35" spans="2:257" s="1" customFormat="1">
+      <c r="B35" s="35"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="IW35" s="2"/>
+    </row>
+    <row r="36" spans="2:257" s="1" customFormat="1">
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="IW36" s="2"/>
+    </row>
+    <row r="37" spans="2:257" s="1" customFormat="1">
+      <c r="B37" s="35"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="IW37" s="2"/>
+    </row>
+    <row r="38" spans="2:257" s="1" customFormat="1">
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="IW38" s="2"/>
+    </row>
+    <row r="39" spans="2:257" s="1" customFormat="1">
+      <c r="B39" s="35"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="IW39" s="2"/>
+    </row>
+    <row r="40" spans="2:257" s="1" customFormat="1">
+      <c r="B40" s="28"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="IW40" s="2"/>
+    </row>
+    <row r="41" spans="2:257" s="1" customFormat="1">
+      <c r="C41" s="28"/>
+      <c r="D41" s="26"/>
+      <c r="IW41" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0" right="0" top="3.9763779527559107E-2" bottom="3.9763779527559107E-2" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="45" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:IW41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2234,32 +2551,32 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
     </row>
     <row r="12" spans="1:257">
       <c r="F12" s="4"/>
@@ -2470,11 +2787,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IW41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2500,32 +2817,32 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
     </row>
     <row r="12" spans="1:257">
       <c r="F12" s="4"/>
@@ -2736,11 +3053,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IW41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2766,32 +3083,32 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
     </row>
     <row r="12" spans="1:257">
       <c r="F12" s="4"/>
@@ -3002,11 +3319,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IW41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -3032,32 +3349,32 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:257">
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:257">
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
     </row>
     <row r="12" spans="1:257">
       <c r="F12" s="4"/>

</xml_diff>